<commit_message>
solução par ao mythril na tradução para dasp
</commit_message>
<xml_diff>
--- a/mythril/0.23.15_smartbugs-curated/0.23.15_slither_smartbugs-curated_dasp.xlsx
+++ b/mythril/0.23.15_smartbugs-curated/0.23.15_slither_smartbugs-curated_dasp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:L1"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,6 +490,1686 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>integer_overflow_mul.sol.json</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>reentrancy_dao.sol.json</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>smart_billions.sol.json</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>simple_suicide.sol.json</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>roulette.sol.json</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>spank_chain_payment.sol.json</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>timelock.sol.json</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>arbitrary_location_write_simple.sol.json</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>eth_tx_order_dependence_minimal.sol.json</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>proxy.sol.json</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>lottery.sol.json</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>rubixi.sol.json</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>integer_overflow_minimal.sol.json</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>modifier_reentrancy.sol.json</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>FibonacciBalance.sol.json</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>wallet_04_confused_sign.sol.json</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>reentrance.sol.json</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>odds_and_evens.sol.json</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>ether_lotto.sol.json</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>integer_overflow_add.sol.json</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>mycontract.sol.json</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>overflow_single_tx.sol.json</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>king_of_the_ether_throne.sol.json</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>reentrancy_simple.sol.json</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>lotto.sol.json</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>etherstore.sol.json</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>crypto_roulette.sol.json</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>integer_overflow_multitx_multifunc_feasible.sol.json</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>wallet_03_wrong_constructor.sol.json</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>token.sol.json</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>integer_overflow_mapping_sym_1.sol.json</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>lucky_doubler.sol.json</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>guess_the_random_number.sol.json</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>wallet_02_refund_nosub.sol.json</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>integer_overflow_multitx_onefunc_feasible.sol.json</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>mapping_write.sol.json</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>list_dos.sol.json</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>integer_overflow_1.sol.json</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>governmental_survey.sol.json</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>old_blockhash.sol.json</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>phishable.sol.json</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>simple_dao.sol.json</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
subindo a analise de teste do smartbugs
</commit_message>
<xml_diff>
--- a/mythril/0.23.15_smartbugs-curated/0.23.15_slither_smartbugs-curated_dasp.xlsx
+++ b/mythril/0.23.15_smartbugs-curated/0.23.15_slither_smartbugs-curated_dasp.xlsx
@@ -500,7 +500,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -592,7 +592,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -604,7 +604,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -678,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -724,7 +724,7 @@
         <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
@@ -740,7 +740,7 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -777,10 +777,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -884,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -912,7 +912,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -964,7 +964,7 @@
         <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13" t="n">
         <v>0</v>
@@ -980,7 +980,7 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -1026,7 +1026,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -1060,13 +1060,13 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -1084,7 +1084,7 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L16" t="n">
         <v>0</v>
@@ -1124,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" t="n">
         <v>0</v>
@@ -1146,10 +1146,10 @@
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -1189,7 +1189,7 @@
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
@@ -1204,7 +1204,7 @@
         <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" t="n">
         <v>0</v>
@@ -1238,13 +1238,13 @@
         <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="n">
         <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20" t="n">
         <v>0</v>
@@ -1260,7 +1260,7 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -1297,7 +1297,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
@@ -1340,7 +1340,7 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -1389,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
@@ -1404,7 +1404,7 @@
         <v>0</v>
       </c>
       <c r="K24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" t="n">
         <v>0</v>
@@ -1426,7 +1426,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -1469,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
@@ -1506,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -1518,7 +1518,7 @@
         <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="n">
         <v>0</v>
@@ -1558,13 +1558,13 @@
         <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="n">
         <v>0</v>
       </c>
       <c r="K28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L28" t="n">
         <v>0</v>
@@ -1580,7 +1580,7 @@
         <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
@@ -1644,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" t="n">
         <v>0</v>
@@ -1660,7 +1660,7 @@
         <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
@@ -1700,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
@@ -1749,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" t="n">
         <v>0</v>
@@ -1777,7 +1777,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
@@ -1844,7 +1844,7 @@
         <v>0</v>
       </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L35" t="n">
         <v>0</v>
@@ -1860,7 +1860,7 @@
         <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" t="n">
         <v>0</v>
@@ -1897,7 +1897,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
@@ -1924,7 +1924,7 @@
         <v>0</v>
       </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L37" t="n">
         <v>0</v>
@@ -1940,7 +1940,7 @@
         <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
@@ -1949,7 +1949,7 @@
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" t="n">
         <v>0</v>
@@ -1958,13 +1958,13 @@
         <v>0</v>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" t="n">
         <v>0</v>
       </c>
       <c r="K38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L38" t="n">
         <v>0</v>
@@ -1980,7 +1980,7 @@
         <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" t="n">
         <v>0</v>
@@ -2026,7 +2026,7 @@
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
@@ -2060,7 +2060,7 @@
         <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" t="n">
         <v>0</v>
@@ -2072,7 +2072,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H41" t="n">
         <v>0</v>
@@ -2097,7 +2097,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
@@ -2146,10 +2146,10 @@
         <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" t="n">
         <v>0</v>

</xml_diff>